<commit_message>
board game + create game template
</commit_message>
<xml_diff>
--- a/WordsContainer.xlsx
+++ b/WordsContainer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\WebstormProjects\CodeName\server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\WebstormProjects\CodeName\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -343,12 +343,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -363,8 +369,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,7 +654,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -657,12 +666,12 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -672,7 +681,7 @@
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -682,7 +691,7 @@
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -692,22 +701,22 @@
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -717,7 +726,7 @@
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -727,12 +736,12 @@
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -747,12 +756,12 @@
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -762,7 +771,7 @@
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -772,22 +781,22 @@
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -797,12 +806,12 @@
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -812,12 +821,12 @@
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>